<commit_message>
update finnish location codes
</commit_message>
<xml_diff>
--- a/inst/extdata/locations_finland_b2020.xlsx
+++ b/inst/extdata/locations_finland_b2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riwh\OneDrive - Folkehelseinstituttet\packages\fhidata\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="13_ncr:1_{E0AA4139-EC72-7240-B4DA-8072FE8D2BA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{D126516D-FC95-43F0-8C50-1A388AC7540D}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="13_ncr:1_{E0AA4139-EC72-7240-B4DA-8072FE8D2BA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{010970E0-62E4-48DB-AE57-032B17DAD15A}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="900" windowWidth="12555" windowHeight="13185" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5805" yWindow="2040" windowWidth="20550" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="norwayLocations" sheetId="1" r:id="rId1"/>
@@ -48,69 +48,6 @@
     <t>Finland</t>
   </si>
   <si>
-    <t>hospitaldistrict09</t>
-  </si>
-  <si>
-    <t>hospitaldistrict15</t>
-  </si>
-  <si>
-    <t>hospitaldistrict10</t>
-  </si>
-  <si>
-    <t>hospitaldistrict25</t>
-  </si>
-  <si>
-    <t>hospitaldistrict11</t>
-  </si>
-  <si>
-    <t>hospitaldistrict19</t>
-  </si>
-  <si>
-    <t>hospitaldistrict05</t>
-  </si>
-  <si>
-    <t>hospitaldistrict17</t>
-  </si>
-  <si>
-    <t>hospitaldistrict14</t>
-  </si>
-  <si>
-    <t>hospitaldistrict08</t>
-  </si>
-  <si>
-    <t>hospitaldistrict21</t>
-  </si>
-  <si>
-    <t>hospitaldistrict20</t>
-  </si>
-  <si>
-    <t>hospitaldistrict06</t>
-  </si>
-  <si>
-    <t>hospitaldistrict12</t>
-  </si>
-  <si>
-    <t>hospitaldistrict18</t>
-  </si>
-  <si>
-    <t>hospitaldistrict13</t>
-  </si>
-  <si>
-    <t>hospitaldistrict07</t>
-  </si>
-  <si>
-    <t>hospitaldistrict04</t>
-  </si>
-  <si>
-    <t>hospitaldistrict16</t>
-  </si>
-  <si>
-    <t>hospitaldistrict03</t>
-  </si>
-  <si>
-    <t>hospitaldistrict00</t>
-  </si>
-  <si>
     <t>FIN</t>
   </si>
   <si>
@@ -178,6 +115,69 @@
   </si>
   <si>
     <t>Varsinais-Suomi Hospital District</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict09</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict15</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict10</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict25</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict11</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict19</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict05</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict17</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict14</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict08</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict21</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict20</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict06</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict12</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict18</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict13</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict07</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict04</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict16</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict03</t>
+  </si>
+  <si>
+    <t>fi_hospitaldistrict00</t>
   </si>
 </sst>
 </file>
@@ -533,7 +533,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D23"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,13 +561,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -575,296 +575,296 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
         <v>28</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
         <v>23</v>
-      </c>
-      <c r="D19" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
       <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
         <v>24</v>
-      </c>
-      <c r="D20" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
       <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
         <v>25</v>
-      </c>
-      <c r="D21" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>